<commit_message>
fix: link color setting
</commit_message>
<xml_diff>
--- a/testfile/link file without stre.xlsx
+++ b/testfile/link file without stre.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Works\FreeCircos\testfile\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2C95FFD-2727-4880-B3F4-3A988DA3AF34}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="30" windowWidth="18210" windowHeight="7320"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13245" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="links" sheetId="1" r:id="rId1"/>
@@ -14,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="21">
   <si>
     <t>Gene1</t>
   </si>
@@ -83,15 +89,11 @@
     <t>lwd</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
-  <si>
-    <t>Stre</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -685,24 +687,24 @@
     </xf>
   </cellXfs>
   <cellStyles count="42">
-    <cellStyle name="20% - 强调文字颜色 1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - 强调文字颜色 2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - 强调文字颜色 3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - 强调文字颜色 4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - 强调文字颜色 5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - 强调文字颜色 6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - 强调文字颜色 1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - 强调文字颜色 2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - 强调文字颜色 3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - 强调文字颜色 4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - 强调文字颜色 5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - 强调文字颜色 6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - 强调文字颜色 1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - 强调文字颜色 2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - 强调文字颜色 3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - 强调文字颜色 4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - 强调文字颜色 5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - 强调文字颜色 6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="20% - 着色 1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - 着色 2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - 着色 3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - 着色 4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - 着色 5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - 着色 6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - 着色 1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - 着色 2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - 着色 3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - 着色 4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - 着色 5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - 着色 6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - 着色 1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - 着色 2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - 着色 3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - 着色 4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - 着色 5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - 着色 6" xfId="41" builtinId="52" customBuiltin="1"/>
     <cellStyle name="标题" xfId="1" builtinId="15" customBuiltin="1"/>
     <cellStyle name="标题 1" xfId="2" builtinId="16" customBuiltin="1"/>
     <cellStyle name="标题 2" xfId="3" builtinId="17" customBuiltin="1"/>
@@ -717,15 +719,15 @@
     <cellStyle name="解释性文本" xfId="16" builtinId="53" customBuiltin="1"/>
     <cellStyle name="警告文本" xfId="14" builtinId="11" customBuiltin="1"/>
     <cellStyle name="链接单元格" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="强调文字颜色 1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="强调文字颜色 2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="强调文字颜色 3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="强调文字颜色 4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="强调文字颜色 5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="强调文字颜色 6" xfId="38" builtinId="49" customBuiltin="1"/>
     <cellStyle name="适中" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="输出" xfId="10" builtinId="21" customBuiltin="1"/>
     <cellStyle name="输入" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="着色 1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="着色 2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="着色 3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="着色 4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="着色 5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="着色 6" xfId="38" builtinId="49" customBuiltin="1"/>
     <cellStyle name="注释" xfId="15" builtinId="10" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -733,6 +735,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -781,7 +786,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -814,9 +819,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -849,6 +871,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1024,25 +1063,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H99"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G99"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M10" sqref="M10"/>
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="9.26953125" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="10.26953125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.26953125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.26953125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.26953125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6" customWidth="1"/>
-    <col min="8" max="8" width="4.26953125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.25" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="10.25" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.25" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.25" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.25" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="4.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1062,13 +1100,10 @@
         <v>19</v>
       </c>
       <c r="G1" t="s">
-        <v>21</v>
-      </c>
-      <c r="H1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -1085,13 +1120,10 @@
         <v>86980758</v>
       </c>
       <c r="G2">
-        <v>41.324221659999999</v>
-      </c>
-      <c r="H2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -1111,13 +1143,10 @@
         <v>38090000</v>
       </c>
       <c r="G3">
-        <v>31.018951940000001</v>
-      </c>
-      <c r="H3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -1131,13 +1160,10 @@
         <v>38088472</v>
       </c>
       <c r="G4">
-        <v>30.69443369</v>
-      </c>
-      <c r="H4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -1151,13 +1177,10 @@
         <v>143060990</v>
       </c>
       <c r="G5">
-        <v>27.495529139999999</v>
-      </c>
-      <c r="H5">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -1171,13 +1194,10 @@
         <v>144407790</v>
       </c>
       <c r="G6">
-        <v>27.25719634</v>
-      </c>
-      <c r="H6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
         <v>2</v>
       </c>
@@ -1191,13 +1211,10 @@
         <v>136504923</v>
       </c>
       <c r="G7">
-        <v>26.668167960000002</v>
-      </c>
-      <c r="H7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
         <v>2</v>
       </c>
@@ -1211,13 +1228,10 @@
         <v>144407790</v>
       </c>
       <c r="G8">
-        <v>26.641113799999999</v>
-      </c>
-      <c r="H8">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
         <v>2</v>
       </c>
@@ -1231,13 +1245,10 @@
         <v>98289997</v>
       </c>
       <c r="G9">
-        <v>26.489053049999999</v>
-      </c>
-      <c r="H9">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
         <v>2</v>
       </c>
@@ -1251,13 +1262,10 @@
         <v>90702781</v>
       </c>
       <c r="G10">
-        <v>26.311669179999999</v>
-      </c>
-      <c r="H10">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
         <v>3</v>
       </c>
@@ -1271,13 +1279,10 @@
         <v>202370997</v>
       </c>
       <c r="G11">
-        <v>26.24086118</v>
-      </c>
-      <c r="H11">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
         <v>2</v>
       </c>
@@ -1291,13 +1296,10 @@
         <v>98288549</v>
       </c>
       <c r="G12">
-        <v>26.237771720000001</v>
-      </c>
-      <c r="H12">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
         <v>2</v>
       </c>
@@ -1311,13 +1313,10 @@
         <v>86980758</v>
       </c>
       <c r="G13">
-        <v>26.20662875</v>
-      </c>
-      <c r="H13">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
         <v>2</v>
       </c>
@@ -1331,13 +1330,10 @@
         <v>144400664</v>
       </c>
       <c r="G14">
-        <v>26.174508970000002</v>
-      </c>
-      <c r="H14">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
         <v>2</v>
       </c>
@@ -1351,13 +1347,10 @@
         <v>98261688</v>
       </c>
       <c r="G15">
-        <v>26.10105553</v>
-      </c>
-      <c r="H15">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
         <v>2</v>
       </c>
@@ -1371,13 +1364,10 @@
         <v>85372128</v>
       </c>
       <c r="G16">
-        <v>25.91578131</v>
-      </c>
-      <c r="H16">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
         <v>2</v>
       </c>
@@ -1391,13 +1381,10 @@
         <v>144400664</v>
       </c>
       <c r="G17">
-        <v>25.518844130000002</v>
-      </c>
-      <c r="H17">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
         <v>2</v>
       </c>
@@ -1411,13 +1398,10 @@
         <v>90704011</v>
       </c>
       <c r="G18">
-        <v>25.490797480000001</v>
-      </c>
-      <c r="H18">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A19" t="s">
         <v>2</v>
       </c>
@@ -1431,13 +1415,10 @@
         <v>144392105</v>
       </c>
       <c r="G19">
-        <v>24.745210310000001</v>
-      </c>
-      <c r="H19">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A20" t="s">
         <v>2</v>
       </c>
@@ -1451,13 +1432,10 @@
         <v>113306765</v>
       </c>
       <c r="G20">
-        <v>24.662740459999998</v>
-      </c>
-      <c r="H20">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A21" t="s">
         <v>2</v>
       </c>
@@ -1471,13 +1449,10 @@
         <v>113309619</v>
       </c>
       <c r="G21">
-        <v>24.562090959999999</v>
-      </c>
-      <c r="H21">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A22" t="s">
         <v>2</v>
       </c>
@@ -1491,13 +1466,10 @@
         <v>144403097</v>
       </c>
       <c r="G22">
-        <v>24.454569169999999</v>
-      </c>
-      <c r="H22">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A23" t="s">
         <v>2</v>
       </c>
@@ -1511,13 +1483,10 @@
         <v>90709741</v>
       </c>
       <c r="G23">
-        <v>24.296536660000001</v>
-      </c>
-      <c r="H23">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A24" t="s">
         <v>2</v>
       </c>
@@ -1531,13 +1500,10 @@
         <v>90744993</v>
       </c>
       <c r="G24">
-        <v>23.940058109999999</v>
-      </c>
-      <c r="H24">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A25" t="s">
         <v>2</v>
       </c>
@@ -1551,13 +1517,10 @@
         <v>144403097</v>
       </c>
       <c r="G25">
-        <v>23.88041423</v>
-      </c>
-      <c r="H25">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A26" t="s">
         <v>2</v>
       </c>
@@ -1571,13 +1534,10 @@
         <v>55731575</v>
       </c>
       <c r="G26">
-        <v>23.662141569999999</v>
-      </c>
-      <c r="H26">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A27" t="s">
         <v>2</v>
       </c>
@@ -1591,13 +1551,10 @@
         <v>136505127</v>
       </c>
       <c r="G27">
-        <v>23.430626090000001</v>
-      </c>
-      <c r="H27">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A28" t="s">
         <v>6</v>
       </c>
@@ -1611,13 +1568,10 @@
         <v>85533571</v>
       </c>
       <c r="G28">
-        <v>23.393941250000001</v>
-      </c>
-      <c r="H28">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A29" t="s">
         <v>2</v>
       </c>
@@ -1631,13 +1585,10 @@
         <v>85538693</v>
       </c>
       <c r="G29">
-        <v>23.393941250000001</v>
-      </c>
-      <c r="H29">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A30" t="s">
         <v>2</v>
       </c>
@@ -1651,13 +1602,10 @@
         <v>98261802</v>
       </c>
       <c r="G30">
-        <v>23.33733659</v>
-      </c>
-      <c r="H30">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A31" t="s">
         <v>2</v>
       </c>
@@ -1671,13 +1619,10 @@
         <v>136509696</v>
       </c>
       <c r="G31">
-        <v>23.331520900000001</v>
-      </c>
-      <c r="H31">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A32" t="s">
         <v>2</v>
       </c>
@@ -1691,13 +1636,10 @@
         <v>136509679</v>
       </c>
       <c r="G32">
-        <v>23.328271910000002</v>
-      </c>
-      <c r="H32">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A33" t="s">
         <v>3</v>
       </c>
@@ -1711,13 +1653,10 @@
         <v>85558538</v>
       </c>
       <c r="G33">
-        <v>23.010550179999999</v>
-      </c>
-      <c r="H33">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A34" t="s">
         <v>2</v>
       </c>
@@ -1731,13 +1670,10 @@
         <v>85533359</v>
       </c>
       <c r="G34">
-        <v>23.00217692</v>
-      </c>
-      <c r="H34">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A35" t="s">
         <v>2</v>
       </c>
@@ -1751,13 +1687,10 @@
         <v>85577613</v>
       </c>
       <c r="G35">
-        <v>22.9788107</v>
-      </c>
-      <c r="H35">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A36" t="s">
         <v>2</v>
       </c>
@@ -1771,13 +1704,10 @@
         <v>143061160</v>
       </c>
       <c r="G36">
-        <v>22.893129460000001</v>
-      </c>
-      <c r="H36">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A37" t="s">
         <v>2</v>
       </c>
@@ -1791,13 +1721,10 @@
         <v>144403167</v>
       </c>
       <c r="G37">
-        <v>22.870954940000001</v>
-      </c>
-      <c r="H37">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A38" t="s">
         <v>2</v>
       </c>
@@ -1811,13 +1738,10 @@
         <v>90690329</v>
       </c>
       <c r="G38">
-        <v>22.55972079</v>
-      </c>
-      <c r="H38">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A39" t="s">
         <v>2</v>
       </c>
@@ -1831,13 +1755,10 @@
         <v>144280799</v>
       </c>
       <c r="G39">
-        <v>22.470697999999999</v>
-      </c>
-      <c r="H39">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A40" t="s">
         <v>2</v>
       </c>
@@ -1851,13 +1772,10 @@
         <v>144281394</v>
       </c>
       <c r="G40">
-        <v>22.470697999999999</v>
-      </c>
-      <c r="H40">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A41" t="s">
         <v>2</v>
       </c>
@@ -1871,13 +1789,10 @@
         <v>144280799</v>
       </c>
       <c r="G41">
-        <v>22.470697999999999</v>
-      </c>
-      <c r="H41">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A42" t="s">
         <v>2</v>
       </c>
@@ -1891,13 +1806,10 @@
         <v>144281394</v>
       </c>
       <c r="G42">
-        <v>22.470697999999999</v>
-      </c>
-      <c r="H42">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A43" t="s">
         <v>2</v>
       </c>
@@ -1911,13 +1823,10 @@
         <v>85625019</v>
       </c>
       <c r="G43">
-        <v>22.292004250000002</v>
-      </c>
-      <c r="H43">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A44" t="s">
         <v>2</v>
       </c>
@@ -1931,13 +1840,10 @@
         <v>85634460</v>
       </c>
       <c r="G44">
-        <v>22.292004250000002</v>
-      </c>
-      <c r="H44">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A45" t="s">
         <v>2</v>
       </c>
@@ -1951,13 +1857,10 @@
         <v>85376492</v>
       </c>
       <c r="G45">
-        <v>22.288277109999999</v>
-      </c>
-      <c r="H45">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A46" t="s">
         <v>2</v>
       </c>
@@ -1971,13 +1874,10 @@
         <v>19953882</v>
       </c>
       <c r="G46">
-        <v>22.26153656</v>
-      </c>
-      <c r="H46">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A47" t="s">
         <v>2</v>
       </c>
@@ -1991,13 +1891,10 @@
         <v>144279640</v>
       </c>
       <c r="G47">
-        <v>22.249877470000001</v>
-      </c>
-      <c r="H47">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A48" t="s">
         <v>2</v>
       </c>
@@ -2011,13 +1908,10 @@
         <v>144279640</v>
       </c>
       <c r="G48">
-        <v>22.249877470000001</v>
-      </c>
-      <c r="H48">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A49" t="s">
         <v>2</v>
       </c>
@@ -2031,13 +1925,10 @@
         <v>85370873</v>
       </c>
       <c r="G49">
-        <v>22.2257751</v>
-      </c>
-      <c r="H49">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A50" t="s">
         <v>2</v>
       </c>
@@ -2051,13 +1942,10 @@
         <v>90638527</v>
       </c>
       <c r="G50">
-        <v>22.112382700000001</v>
-      </c>
-      <c r="H50">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A51" t="s">
         <v>2</v>
       </c>
@@ -2071,13 +1959,10 @@
         <v>85602225</v>
       </c>
       <c r="G51">
-        <v>22.089962880000002</v>
-      </c>
-      <c r="H51">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A52" t="s">
         <v>2</v>
       </c>
@@ -2091,13 +1976,10 @@
         <v>85371838</v>
       </c>
       <c r="G52">
-        <v>22.08666307</v>
-      </c>
-      <c r="H52">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A53" t="s">
         <v>2</v>
       </c>
@@ -2111,13 +1993,10 @@
         <v>90663670</v>
       </c>
       <c r="G53">
-        <v>22.044312250000001</v>
-      </c>
-      <c r="H53">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A54" t="s">
         <v>2</v>
       </c>
@@ -2131,13 +2010,10 @@
         <v>90664794</v>
       </c>
       <c r="G54">
-        <v>22.044312250000001</v>
-      </c>
-      <c r="H54">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A55" t="s">
         <v>2</v>
       </c>
@@ -2151,13 +2027,10 @@
         <v>90671287</v>
       </c>
       <c r="G55">
-        <v>22.044312250000001</v>
-      </c>
-      <c r="H55">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A56" t="s">
         <v>2</v>
       </c>
@@ -2171,13 +2044,10 @@
         <v>90674451</v>
       </c>
       <c r="G56">
-        <v>22.044312250000001</v>
-      </c>
-      <c r="H56">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A57" t="s">
         <v>2</v>
       </c>
@@ -2191,13 +2061,10 @@
         <v>90675238</v>
       </c>
       <c r="G57">
-        <v>22.044312250000001</v>
-      </c>
-      <c r="H57">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A58" t="s">
         <v>2</v>
       </c>
@@ -2211,13 +2078,10 @@
         <v>144278095</v>
       </c>
       <c r="G58">
-        <v>22.037110009999999</v>
-      </c>
-      <c r="H58">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A59" t="s">
         <v>2</v>
       </c>
@@ -2231,13 +2095,10 @@
         <v>144278095</v>
       </c>
       <c r="G59">
-        <v>22.037110009999999</v>
-      </c>
-      <c r="H59">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A60" t="s">
         <v>2</v>
       </c>
@@ -2251,13 +2112,10 @@
         <v>90638614</v>
       </c>
       <c r="G60">
-        <v>22.00121773</v>
-      </c>
-      <c r="H60">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A61" t="s">
         <v>2</v>
       </c>
@@ -2271,13 +2129,10 @@
         <v>90639847</v>
       </c>
       <c r="G61">
-        <v>22.00121773</v>
-      </c>
-      <c r="H61">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A62" t="s">
         <v>2</v>
       </c>
@@ -2291,13 +2146,10 @@
         <v>136515330</v>
       </c>
       <c r="G62">
-        <v>21.981299499999999</v>
-      </c>
-      <c r="H62">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A63" t="s">
         <v>2</v>
       </c>
@@ -2311,13 +2163,10 @@
         <v>90657491</v>
       </c>
       <c r="G63">
-        <v>21.972650389999998</v>
-      </c>
-      <c r="H63">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A64" t="s">
         <v>2</v>
       </c>
@@ -2331,13 +2180,10 @@
         <v>85597454</v>
       </c>
       <c r="G64">
-        <v>21.95039439</v>
-      </c>
-      <c r="H64">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A65" t="s">
         <v>2</v>
       </c>
@@ -2351,13 +2197,10 @@
         <v>85682637</v>
       </c>
       <c r="G65">
-        <v>21.797239309999998</v>
-      </c>
-      <c r="H65">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A66" t="s">
         <v>2</v>
       </c>
@@ -2371,13 +2214,10 @@
         <v>90624787</v>
       </c>
       <c r="G66">
-        <v>21.791021480000001</v>
-      </c>
-      <c r="H66">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A67" t="s">
         <v>2</v>
       </c>
@@ -2391,13 +2231,10 @@
         <v>85264266</v>
       </c>
       <c r="G67">
-        <v>21.77989191</v>
-      </c>
-      <c r="H67">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A68" t="s">
         <v>2</v>
       </c>
@@ -2411,13 +2248,10 @@
         <v>55731575</v>
       </c>
       <c r="G68">
-        <v>21.73259358</v>
-      </c>
-      <c r="H68">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A69" t="s">
         <v>2</v>
       </c>
@@ -2431,13 +2265,10 @@
         <v>90639515</v>
       </c>
       <c r="G69">
-        <v>21.72376804</v>
-      </c>
-      <c r="H69">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A70" t="s">
         <v>2</v>
       </c>
@@ -2451,13 +2282,10 @@
         <v>85372128</v>
       </c>
       <c r="G70">
-        <v>21.71919407</v>
-      </c>
-      <c r="H70">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A71" t="s">
         <v>2</v>
       </c>
@@ -2471,13 +2299,10 @@
         <v>85682637</v>
       </c>
       <c r="G71">
-        <v>21.609241470000001</v>
-      </c>
-      <c r="H71">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A72" t="s">
         <v>2</v>
       </c>
@@ -2491,13 +2316,10 @@
         <v>144390067</v>
       </c>
       <c r="G72">
-        <v>21.58838029</v>
-      </c>
-      <c r="H72">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A73" t="s">
         <v>2</v>
       </c>
@@ -2511,13 +2333,10 @@
         <v>85315738</v>
       </c>
       <c r="G73">
-        <v>21.391260079999999</v>
-      </c>
-      <c r="H73">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A74" t="s">
         <v>2</v>
       </c>
@@ -2531,13 +2350,10 @@
         <v>19953882</v>
       </c>
       <c r="G74">
-        <v>21.244353780000001</v>
-      </c>
-      <c r="H74">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A75" t="s">
         <v>2</v>
       </c>
@@ -2551,13 +2367,10 @@
         <v>85653433</v>
       </c>
       <c r="G75">
-        <v>21.184422250000001</v>
-      </c>
-      <c r="H75">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A76" t="s">
         <v>2</v>
       </c>
@@ -2571,13 +2384,10 @@
         <v>136515330</v>
       </c>
       <c r="G76">
-        <v>21.177701129999999</v>
-      </c>
-      <c r="H76">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A77" t="s">
         <v>2</v>
       </c>
@@ -2591,13 +2401,10 @@
         <v>144390067</v>
       </c>
       <c r="G77">
-        <v>21.08698132</v>
-      </c>
-      <c r="H77">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A78" t="s">
         <v>2</v>
       </c>
@@ -2611,13 +2418,10 @@
         <v>85653433</v>
       </c>
       <c r="G78">
-        <v>20.990974260000002</v>
-      </c>
-      <c r="H78">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A79" t="s">
         <v>2</v>
       </c>
@@ -2631,13 +2435,10 @@
         <v>85653433</v>
       </c>
       <c r="G79">
-        <v>20.990974260000002</v>
-      </c>
-      <c r="H79">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A80" t="s">
         <v>2</v>
       </c>
@@ -2651,13 +2452,10 @@
         <v>143197975</v>
       </c>
       <c r="G80">
-        <v>20.50403961</v>
-      </c>
-      <c r="H80">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A81" t="s">
         <v>2</v>
       </c>
@@ -2671,13 +2469,10 @@
         <v>1377021</v>
       </c>
       <c r="G81">
-        <v>20.4015378</v>
-      </c>
-      <c r="H81">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A82" t="s">
         <v>2</v>
       </c>
@@ -2691,13 +2486,10 @@
         <v>90675238</v>
       </c>
       <c r="G82">
-        <v>19.712422190000002</v>
-      </c>
-      <c r="H82">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A83" t="s">
         <v>2</v>
       </c>
@@ -2711,13 +2503,10 @@
         <v>55730124</v>
       </c>
       <c r="G83">
-        <v>19.680269509999999</v>
-      </c>
-      <c r="H83">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A84" t="s">
         <v>2</v>
       </c>
@@ -2731,13 +2520,10 @@
         <v>90638614</v>
       </c>
       <c r="G84">
-        <v>19.675100499999999</v>
-      </c>
-      <c r="H84">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A85" t="s">
         <v>2</v>
       </c>
@@ -2751,13 +2537,10 @@
         <v>90639847</v>
       </c>
       <c r="G85">
-        <v>19.675100499999999</v>
-      </c>
-      <c r="H85">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A86" t="s">
         <v>2</v>
       </c>
@@ -2771,13 +2554,10 @@
         <v>1377172</v>
       </c>
       <c r="G86">
-        <v>19.59585075</v>
-      </c>
-      <c r="H86">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A87" t="s">
         <v>2</v>
       </c>
@@ -2791,13 +2571,10 @@
         <v>143170004</v>
       </c>
       <c r="G87">
-        <v>19.548213560000001</v>
-      </c>
-      <c r="H87">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A88" t="s">
         <v>2</v>
       </c>
@@ -2811,13 +2588,10 @@
         <v>90709741</v>
       </c>
       <c r="G88">
-        <v>16.169539650000001</v>
-      </c>
-      <c r="H88">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A89" t="s">
         <v>2</v>
       </c>
@@ -2831,13 +2605,10 @@
         <v>136519258</v>
       </c>
       <c r="G89">
-        <v>16.16071054</v>
-      </c>
-      <c r="H89">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A90" t="s">
         <v>2</v>
       </c>
@@ -2851,13 +2622,10 @@
         <v>90764310</v>
       </c>
       <c r="G90">
-        <v>16.04114955</v>
-      </c>
-      <c r="H90">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A91" t="s">
         <v>2</v>
       </c>
@@ -2871,13 +2639,10 @@
         <v>136522274</v>
       </c>
       <c r="G91">
-        <v>15.85232368</v>
-      </c>
-      <c r="H91">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A92" t="s">
         <v>2</v>
       </c>
@@ -2891,13 +2656,10 @@
         <v>174863690</v>
       </c>
       <c r="G92">
-        <v>15.743763469999999</v>
-      </c>
-      <c r="H92">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A93" t="s">
         <v>2</v>
       </c>
@@ -2911,13 +2673,10 @@
         <v>98302136</v>
       </c>
       <c r="G93">
-        <v>15.7235382</v>
-      </c>
-      <c r="H93">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A94" t="s">
         <v>2</v>
       </c>
@@ -2931,13 +2690,10 @@
         <v>90704011</v>
       </c>
       <c r="G94">
-        <v>15.598944270000001</v>
-      </c>
-      <c r="H94">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A95" t="s">
         <v>2</v>
       </c>
@@ -2951,13 +2707,10 @@
         <v>136519639</v>
       </c>
       <c r="G95">
-        <v>15.07381195</v>
-      </c>
-      <c r="H95">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A96" t="s">
         <v>2</v>
       </c>
@@ -2971,13 +2724,10 @@
         <v>119091401</v>
       </c>
       <c r="G96">
-        <v>14.67039875</v>
-      </c>
-      <c r="H96">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A97" t="s">
         <v>2</v>
       </c>
@@ -2991,13 +2741,10 @@
         <v>55726462</v>
       </c>
       <c r="G97">
-        <v>14.528121799999999</v>
-      </c>
-      <c r="H97">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A98" t="s">
         <v>2</v>
       </c>
@@ -3011,13 +2758,10 @@
         <v>144318529</v>
       </c>
       <c r="G98">
-        <v>14.50237935</v>
-      </c>
-      <c r="H98">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A99" t="s">
         <v>2</v>
       </c>
@@ -3031,9 +2775,6 @@
         <v>136509448</v>
       </c>
       <c r="G99">
-        <v>14.49241396</v>
-      </c>
-      <c r="H99">
         <v>2</v>
       </c>
     </row>

</xml_diff>